<commit_message>
Updated document and src folder
</commit_message>
<xml_diff>
--- a/documents/Published/Trading Chart/TradingChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Trading Chart/TradingChartByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18518"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\TradingChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{999A6BCD-540E-41A8-ABAF-EAFE90DC1D72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="7965" xr2:uid="{6D425234-7E7F-490C-8907-5B869BB20B46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D425234-7E7F-490C-8907-5B869BB20B46}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>S no</t>
   </si>
@@ -297,6 +298,18 @@
   </si>
   <si>
     <t>Does visual legends adjusted on resizing? </t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>Internet Explorer</t>
+  </si>
+  <si>
+    <t>Desktop</t>
   </si>
 </sst>
 </file>
@@ -428,24 +441,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -464,6 +459,24 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,6 +492,1243 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3557604</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1495425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0768C12E-32FB-45BE-8657-F06EA4AA01AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12763500" y="295275"/>
+          <a:ext cx="3090879" cy="1390650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3596737</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1524000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{058D0426-1D9A-4A44-9752-CCFE168020A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10267949" y="295276"/>
+          <a:ext cx="3320513" cy="1419224"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3634838</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1571624</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F659196-7DEC-448C-810F-CCF2649330F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14173200" y="342900"/>
+          <a:ext cx="3320513" cy="1419224"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3672938</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1533524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DF00596-08D2-4DFA-9426-C673D42B7A20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17907000" y="304800"/>
+          <a:ext cx="3320513" cy="1419224"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>145742</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3962400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1578685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8A85933-980F-4600-9462-DBAFB639E5ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22955251" y="2050742"/>
+          <a:ext cx="3467099" cy="1432943"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371477</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50492</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3905250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1615091</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F8E60FE-079B-4569-8CE5-DE8C043C8421}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17926052" y="1955492"/>
+          <a:ext cx="3533773" cy="1564599"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3657598</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1621749</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D70EDD8E-2527-4935-A8D2-776B4DCC7DCD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13982700" y="1962150"/>
+          <a:ext cx="3533773" cy="1564599"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3771898</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1640799</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3FCE86C-3ECE-4EF4-94C5-0BA04E8C6E2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10229850" y="1981200"/>
+          <a:ext cx="3533773" cy="1564599"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>523617</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4544897</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1790700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B99CB09E-3F03-4BF3-89CB-0051548E5346}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22983567" y="3771901"/>
+          <a:ext cx="4021280" cy="1638299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4516580</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1809749</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{285D2430-CE22-4032-ABEF-1827DC1F0BEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18049875" y="3790950"/>
+          <a:ext cx="4021280" cy="1638299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4392755</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1657349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A818D20-7D7D-4F65-9078-AFEC23B1A7B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14230350" y="3638550"/>
+          <a:ext cx="4021280" cy="1638299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4249880</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1714499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB62259B-FFFA-4F85-A41E-28A86848DD0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10220325" y="3695700"/>
+          <a:ext cx="4021280" cy="1638299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3799272</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1600200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACA5697F-6E3A-45E9-BF25-68A29FE159A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24364950" y="5676900"/>
+          <a:ext cx="3446847" cy="1438275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4362450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1723014</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D21D486-A603-4D51-AA61-EE3CBF720C9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19488150" y="5514975"/>
+          <a:ext cx="3981450" cy="1723014"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3914775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1631770</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BCBD2EA-4C01-4F53-91B0-4F5888F40C6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14801850" y="5572125"/>
+          <a:ext cx="3638550" cy="1574620"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3924300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1611883</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC79CA30-E875-4A28-86B4-7BB15660E938}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10477500" y="5638800"/>
+          <a:ext cx="3438525" cy="1488058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4133850</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1895427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D45702C6-35E3-4DA1-AD1F-C6FED6085F83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24469725" y="7324726"/>
+          <a:ext cx="3676650" cy="1838276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>128025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3978999</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1714500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7780DA3-5155-4CED-AB3D-1C27BFA3C666}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10315575" y="7395600"/>
+          <a:ext cx="3655149" cy="1586475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4045674</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1748400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B595E6-829F-41F4-93D0-FC9482981BA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14916150" y="7429500"/>
+          <a:ext cx="3655149" cy="1586475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4121874</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1757925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEBE1F15-CC9A-44BA-B47B-AAFEE58A427E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19573875" y="7439025"/>
+          <a:ext cx="3655149" cy="1586475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>203955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3971925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1753728</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8CE426F-7F89-4968-AC98-39A768A66AAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24269700" y="9405105"/>
+          <a:ext cx="3714750" cy="1549773"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4733925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2002815</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71F8E006-2ACD-4207-ADF8-1D6E8E501291}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19354800" y="9305925"/>
+          <a:ext cx="4486275" cy="1898040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4572000</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2012340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2F0F614-35D4-4AA2-9B83-25E71345B638}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14611350" y="9315450"/>
+          <a:ext cx="4486275" cy="1898040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2012340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D1F5405-F170-41F2-957A-7F18367E4FD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10039350" y="9315450"/>
+          <a:ext cx="4486275" cy="1898040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4114800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1896249</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98AAF099-73B5-484F-BFD9-AC63628A9242}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10487025" y="11620500"/>
+          <a:ext cx="3829050" cy="1572399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4578649</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2076451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF5C17CA-9DCC-40BD-B92C-20042BA14A75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14830425" y="11449051"/>
+          <a:ext cx="4483399" cy="1924050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4750099</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2085975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2178D5A-D241-4A87-9C6E-03C9C2666BC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19583400" y="11458575"/>
+          <a:ext cx="4483399" cy="1924050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>4769149</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2105025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E48EC481-49CF-4C7D-BC56-78F599DBABC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24507825" y="11477625"/>
+          <a:ext cx="4483399" cy="1924050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -778,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2FE1A9-DE58-4E51-9284-DEF7424B442C}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,10 +2039,14 @@
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="41.28515625" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68" customWidth="1"/>
+    <col min="7" max="7" width="68.7109375" customWidth="1"/>
+    <col min="8" max="8" width="73.5703125" customWidth="1"/>
+    <col min="9" max="9" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,8 +2062,20 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -826,7 +2092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -843,7 +2109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -860,7 +2126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -877,7 +2143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -894,7 +2160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -911,7 +2177,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -930,6 +2196,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1123,29 +2390,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="16" t="s">
+      <c r="A18" s="13"/>
+      <c r="B18" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="14"/>
+      <c r="B19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
@@ -1159,41 +2426,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="12">
         <v>18</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="13"/>
+      <c r="B22" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="13" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">

</xml_diff>